<commit_message>
Novo desafio de estagio
</commit_message>
<xml_diff>
--- a/Planilhas_Metas.xlsx
+++ b/Planilhas_Metas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Documents\Desenvolvimento 2022\Excel Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902A6A97-B7CB-43DE-B269-A384EF7ECE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC6EDE6-6C72-4BF2-9B38-861B15131C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{23C04C42-1C65-4DBB-920C-11ED9BB55231}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{23C04C42-1C65-4DBB-920C-11ED9BB55231}"/>
   </bookViews>
   <sheets>
     <sheet name="Janeiro" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="28">
   <si>
     <t>Meta</t>
   </si>
@@ -111,6 +113,12 @@
   </si>
   <si>
     <t>melhorar o quarto</t>
+  </si>
+  <si>
+    <t>Reduzir a conta de internet</t>
+  </si>
+  <si>
+    <t>Reduzir os custos</t>
   </si>
 </sst>
 </file>
@@ -160,12 +168,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -249,52 +257,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -307,26 +270,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -340,19 +290,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -363,7 +300,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -372,72 +309,31 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -539,11 +435,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -553,162 +554,163 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+  <dxfs count="29">
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="medium">
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
@@ -719,13 +721,11 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -742,7 +742,9 @@
         <left style="medium">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -754,11 +756,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -771,18 +770,17 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -790,102 +788,15 @@
         <left style="medium">
           <color indexed="64"/>
         </left>
-        <right style="medium">
+        <right style="thin">
           <color indexed="64"/>
         </right>
         <top style="medium">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -977,6 +888,193 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -992,14 +1090,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB86D063-0FB2-4EA5-96A6-B2822A4F527C}" name="Tabela1" displayName="Tabela1" ref="L2:P12" totalsRowShown="0" dataDxfId="6" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB86D063-0FB2-4EA5-96A6-B2822A4F527C}" name="Tabela1" displayName="Tabela1" ref="L2:P12" totalsRowShown="0" dataDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="L2:P12" xr:uid="{CB86D063-0FB2-4EA5-96A6-B2822A4F527C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A357CE9A-AD42-4066-950D-9F046D1DE654}" name="Meta" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{B8AE6149-793B-40A1-BE92-88197D6E55D1}" name="Progresso" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{09348D36-0C8D-42B4-AD81-7F860EB3E994}" name="Observação" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{EC72D661-28FE-4B61-9462-35B357CF8EA7}" name="Prazo" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{EF098A3D-F5EB-45CE-A7F6-81BBD397A439}" name="Status" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{A357CE9A-AD42-4066-950D-9F046D1DE654}" name="Meta" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{B8AE6149-793B-40A1-BE92-88197D6E55D1}" name="Progresso" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{09348D36-0C8D-42B4-AD81-7F860EB3E994}" name="Observação" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{EC72D661-28FE-4B61-9462-35B357CF8EA7}" name="Prazo" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{EF098A3D-F5EB-45CE-A7F6-81BBD397A439}" name="Status" dataDxfId="22">
       <calculatedColumnFormula>CHOOSE(MATCH(M3,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1008,18 +1106,31 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F2083493-6C53-4CBC-8D0D-DC5010409185}" name="Tabela2" displayName="Tabela2" ref="L17:P27" totalsRowShown="0" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F2083493-6C53-4CBC-8D0D-DC5010409185}" name="Tabela2" displayName="Tabela2" ref="L17:P27" totalsRowShown="0" tableBorderDxfId="21">
   <autoFilter ref="L17:P27" xr:uid="{F2083493-6C53-4CBC-8D0D-DC5010409185}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9BE76760-57D1-4307-9194-D9336995FB1E}" name="Meta" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{BA81C0E7-4DA5-4C39-9CBB-0C6860D732A7}" name="Progresso" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{F789F8F4-0B10-4A93-BF91-124142485D55}" name="Observação" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{E0295F28-1C49-4E5E-A09D-0AAF302FB8C0}" name="Prazo" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{10891836-39D1-40A9-A138-E4D1CA28A2D5}" name="Status" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{9BE76760-57D1-4307-9194-D9336995FB1E}" name="Meta" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{BA81C0E7-4DA5-4C39-9CBB-0C6860D732A7}" name="Progresso" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{F789F8F4-0B10-4A93-BF91-124142485D55}" name="Observação" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{E0295F28-1C49-4E5E-A09D-0AAF302FB8C0}" name="Prazo" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{10891836-39D1-40A9-A138-E4D1CA28A2D5}" name="Status" dataDxfId="16">
       <calculatedColumnFormula>CHOOSE(MATCH(M18,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CD0A6FD6-A655-48AC-B5B2-206867A18123}" name="Tabela6" displayName="Tabela6" ref="D17:G27" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="D17:G27" xr:uid="{CD0A6FD6-A655-48AC-B5B2-206867A18123}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A73B7E0D-9423-4D6C-B912-916DB3D84954}" name="Meta" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{38854C7E-677C-4848-AABA-031E507AC936}" name="Progresso" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{A4BCD98C-E2FF-4F57-ABB1-694512FC29FD}" name="Observação" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{EDCE1AE8-90E0-4DC6-84DA-A5CAB83FECAB}" name="Prazo" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1322,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D22F7A3-C2CF-46BF-A49B-98FCFD9603D7}">
   <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F9" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,7 +1442,7 @@
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
@@ -1345,324 +1456,324 @@
   <sheetData>
     <row r="1" spans="2:16" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="50" t="s">
+      <c r="K2" s="37"/>
+      <c r="L2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="51" t="s">
+      <c r="M2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="52" t="s">
+      <c r="N2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="53" t="s">
+      <c r="O2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="53" t="s">
+      <c r="P2" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="23">
-        <v>44941</v>
-      </c>
-      <c r="H3" s="13" t="str">
+      <c r="G3" s="15">
+        <v>44943</v>
+      </c>
+      <c r="H3" s="8" t="str">
         <f>CHOOSE(MATCH(E3,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Ok</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="54" t="s">
+      <c r="J3" s="38"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="7" t="s">
+      <c r="M3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="7" t="str">
+      <c r="O3" s="15"/>
+      <c r="P3" s="4" t="str">
         <f>CHOOSE(MATCH(M3,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="13" t="str">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="8" t="str">
         <f>CHOOSE(MATCH(E4,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="54" t="s">
+      <c r="J4" s="38"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" s="18"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="7" t="str">
+      <c r="M4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="4" t="str">
         <f>CHOOSE(MATCH(M4,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="18" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="13" t="str">
+      <c r="F5" s="5"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="8" t="str">
         <f>CHOOSE(MATCH(E5,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Ok</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="18" t="s">
+      <c r="J5" s="38"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="18"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="7" t="str">
+      <c r="N5" s="10"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="4" t="str">
         <f>CHOOSE(MATCH(M5,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Ok</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="13" t="str">
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="8" t="str">
         <f>CHOOSE(MATCH(E6,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N6" s="18"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="7" t="str">
+      <c r="J6" s="38"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="10"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="4" t="str">
         <f>CHOOSE(MATCH(M6,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="13" t="str">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="8" t="str">
         <f>CHOOSE(MATCH(E7,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="7" t="str">
+      <c r="J7" s="38"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="10"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="4" t="str">
         <f>CHOOSE(MATCH(M7,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="13" t="str">
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="8" t="str">
         <f>CHOOSE(MATCH(E8,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N8" s="18"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="7" t="str">
+      <c r="J8" s="38"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="4" t="str">
         <f>CHOOSE(MATCH(M8,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="13" t="str">
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="8" t="str">
         <f>CHOOSE(MATCH(E9,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="7" t="str">
+      <c r="J9" s="38"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="4" t="str">
         <f>CHOOSE(MATCH(M9,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="13" t="str">
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="8" t="str">
         <f>CHOOSE(MATCH(E10,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N10" s="18"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="7" t="str">
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="10"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="4" t="str">
         <f>CHOOSE(MATCH(M10,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="28"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="13" t="str">
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="8" t="str">
         <f>CHOOSE(MATCH(E11,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N11" s="18"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="7" t="str">
+      <c r="J11" s="38"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="10"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="4" t="str">
         <f>CHOOSE(MATCH(M11,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="13" t="str">
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="8" t="str">
         <f>CHOOSE(MATCH(E12,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="7" t="str">
+      <c r="J12" s="40"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="11"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="4" t="str">
         <f>CHOOSE(MATCH(M12,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
@@ -1687,294 +1798,300 @@
     </row>
     <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="44" t="s">
+      <c r="J17" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="45"/>
-      <c r="L17" s="50" t="s">
+      <c r="K17" s="43"/>
+      <c r="L17" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="M17" s="51" t="s">
+      <c r="M17" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="N17" s="52" t="s">
+      <c r="N17" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="O17" s="53" t="s">
+      <c r="O17" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="P17" s="53" t="s">
+      <c r="P17" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="18" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="11" t="s">
+      <c r="E18" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="14" t="str">
+      <c r="H18" s="50" t="str">
         <f>IF(E18="Não Feito", "Burro", IF(E18="Fazendo", "Ok", IF(E18="Completo", "Tu é Pika")))</f>
         <v>Tu é Pika</v>
       </c>
-      <c r="J18" s="46"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="54" t="s">
+      <c r="J18" s="44"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="18" t="s">
+      <c r="M18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="N18" s="7" t="s">
+      <c r="N18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O18" s="23"/>
-      <c r="P18" s="7" t="str">
+      <c r="O18" s="15"/>
+      <c r="P18" s="4" t="str">
         <f>CHOOSE(MATCH(M18,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Burro</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="16" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="11"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="14"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="54" t="s">
+      <c r="H19" s="50"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="18" t="s">
+      <c r="M19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="18" t="s">
+      <c r="N19" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="24">
+      <c r="O19" s="16">
         <v>45311</v>
       </c>
-      <c r="P19" s="7" t="str">
+      <c r="P19" s="4" t="str">
         <f>CHOOSE(MATCH(M19,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Burro</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="34"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="16" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="11"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="14"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="54" t="s">
+      <c r="H20" s="50"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="M20" s="18" t="s">
+      <c r="M20" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="N20" s="18" t="s">
+      <c r="N20" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="O20" s="24">
+      <c r="O20" s="16">
         <v>45304</v>
       </c>
-      <c r="P20" s="7" t="str">
+      <c r="P20" s="4" t="str">
         <f>CHOOSE(MATCH(M20,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Burro</v>
       </c>
     </row>
     <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="11"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="7"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="14"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N21" s="18"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="7" t="str">
+      <c r="H21" s="50"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O21" s="16">
+        <v>45308</v>
+      </c>
+      <c r="P21" s="4" t="str">
         <f>CHOOSE(MATCH(M21,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
-        <v>Tu é Pika</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="11"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="7"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="14"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N22" s="18"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="7" t="str">
+      <c r="H22" s="50"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N22" s="10"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="4" t="str">
         <f>CHOOSE(MATCH(M22,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="11"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="7"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="14"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N23" s="18"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="7" t="str">
+      <c r="H23" s="50"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" s="10"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="4" t="str">
         <f>CHOOSE(MATCH(M23,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="34"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="11"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="7"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="14"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N24" s="18"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="7" t="str">
+      <c r="H24" s="50"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N24" s="10"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="4" t="str">
         <f>CHOOSE(MATCH(M24,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="11"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="7"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="14"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N25" s="18"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="7" t="str">
+      <c r="H25" s="50"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" s="10"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="4" t="str">
         <f>CHOOSE(MATCH(M25,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="11"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="7"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="14"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="N26" s="18"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="7" t="str">
+      <c r="H26" s="50"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N26" s="10"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="4" t="str">
         <f>CHOOSE(MATCH(M26,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="15"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="N27" s="19"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="7" t="str">
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="56"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="51"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N27" s="11"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="4" t="str">
         <f>CHOOSE(MATCH(M27,{"Não Feito";"Fazendo";"Completo"},0), "Burro", "Ok", "Tu é Pika")</f>
         <v>Tu é Pika</v>
       </c>
@@ -1987,35 +2104,35 @@
     <mergeCell ref="J17:K27"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H12">
-    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="Tu é Pika">
+    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="Tu é Pika">
       <formula>NOT(ISERROR(SEARCH("Tu é Pika",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="8" operator="containsText" text="Burro">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="Burro">
       <formula>NOT(ISERROR(SEARCH("Burro",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P12">
-    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="Tu é Pika">
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Tu é Pika">
       <formula>NOT(ISERROR(SEARCH("Tu é Pika",P3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="Burro">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Burro">
       <formula>NOT(ISERROR(SEARCH("Burro",P3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",P3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18:P27">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Tu é Pika">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Tu é Pika">
       <formula>NOT(ISERROR(SEARCH("Tu é Pika",P18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Burro">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Burro">
       <formula>NOT(ISERROR(SEARCH("Burro",P18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",P18)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2029,9 +2146,10 @@
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>